<commit_message>
saved work Friday before take trip -__-
</commit_message>
<xml_diff>
--- a/BWTracker.xlsx
+++ b/BWTracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="105">
   <si>
     <t>day</t>
   </si>
@@ -282,12 +282,60 @@
   </si>
   <si>
     <t>03:27:44</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>00:56:12</t>
+  </si>
+  <si>
+    <t>detailed state diagram</t>
+  </si>
+  <si>
+    <t>00:50:13</t>
+  </si>
+  <si>
+    <t>Clone TamCustomOSForPi</t>
+  </si>
+  <si>
+    <t>clone + store</t>
+  </si>
+  <si>
+    <t>00:05:31</t>
+  </si>
+  <si>
+    <t>00:18:58</t>
+  </si>
+  <si>
+    <t>Pi 5.8 Deployment Library</t>
+  </si>
+  <si>
+    <t>investigate http://doc.qt.io/qt-5/windows-deployment.html + try to make binary file qt 5.8 run on Pi with qt 5.3 via standalone library file</t>
+  </si>
+  <si>
+    <t>00:35:33</t>
+  </si>
+  <si>
+    <t>02:31:07</t>
+  </si>
+  <si>
+    <t>00:44:55</t>
+  </si>
+  <si>
+    <t>QtAppSelfContainerGenerator</t>
+  </si>
+  <si>
+    <t>directly write a console application</t>
+  </si>
+  <si>
+    <t>00:35:25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,6 +538,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -525,6 +590,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -702,7 +784,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:EL42"/>
+  <dimension ref="A1:EL50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
@@ -3455,6 +3537,454 @@
         <v>22</v>
       </c>
     </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="2">
+        <v>16</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E43" s="2">
+        <v>24</v>
+      </c>
+      <c r="F43" s="2">
+        <v>7</v>
+      </c>
+      <c r="G43" s="2">
+        <v>22</v>
+      </c>
+      <c r="H43" s="2">
+        <v>13</v>
+      </c>
+      <c r="I43" s="2">
+        <v>8</v>
+      </c>
+      <c r="J43" s="2">
+        <v>18</v>
+      </c>
+      <c r="K43" s="2">
+        <v>26</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q43" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R43" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="2">
+        <v>16</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E44" s="2">
+        <v>24</v>
+      </c>
+      <c r="F44" s="2">
+        <v>8</v>
+      </c>
+      <c r="G44" s="2">
+        <v>18</v>
+      </c>
+      <c r="H44" s="2">
+        <v>38</v>
+      </c>
+      <c r="I44" s="2">
+        <v>9</v>
+      </c>
+      <c r="J44" s="2">
+        <v>8</v>
+      </c>
+      <c r="K44" s="2">
+        <v>51</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R44" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="2">
+        <v>16</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E45" s="2">
+        <v>24</v>
+      </c>
+      <c r="F45" s="2">
+        <v>9</v>
+      </c>
+      <c r="G45" s="2">
+        <v>10</v>
+      </c>
+      <c r="H45" s="2">
+        <v>6</v>
+      </c>
+      <c r="I45" s="2">
+        <v>9</v>
+      </c>
+      <c r="J45" s="2">
+        <v>15</v>
+      </c>
+      <c r="K45" s="2">
+        <v>38</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B46" s="2">
+        <v>16</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E46" s="2">
+        <v>24</v>
+      </c>
+      <c r="F46" s="2">
+        <v>9</v>
+      </c>
+      <c r="G46" s="2">
+        <v>27</v>
+      </c>
+      <c r="H46" s="2">
+        <v>3</v>
+      </c>
+      <c r="I46" s="2">
+        <v>9</v>
+      </c>
+      <c r="J46" s="2">
+        <v>46</v>
+      </c>
+      <c r="K46" s="2">
+        <v>2</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R46" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="2">
+        <v>16</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E47" s="2">
+        <v>24</v>
+      </c>
+      <c r="F47" s="2">
+        <v>9</v>
+      </c>
+      <c r="G47" s="2">
+        <v>48</v>
+      </c>
+      <c r="H47" s="2">
+        <v>38</v>
+      </c>
+      <c r="I47" s="2">
+        <v>10</v>
+      </c>
+      <c r="J47" s="2">
+        <v>24</v>
+      </c>
+      <c r="K47" s="2">
+        <v>12</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R47" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="2">
+        <v>16</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E48" s="2">
+        <v>24</v>
+      </c>
+      <c r="F48" s="2">
+        <v>10</v>
+      </c>
+      <c r="G48" s="2">
+        <v>39</v>
+      </c>
+      <c r="H48" s="2">
+        <v>44</v>
+      </c>
+      <c r="I48" s="2">
+        <v>13</v>
+      </c>
+      <c r="J48" s="2">
+        <v>10</v>
+      </c>
+      <c r="K48" s="2">
+        <v>52</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N48" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="2">
+        <v>16</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E49" s="2">
+        <v>24</v>
+      </c>
+      <c r="F49" s="2">
+        <v>14</v>
+      </c>
+      <c r="G49" s="2">
+        <v>8</v>
+      </c>
+      <c r="H49" s="2">
+        <v>3</v>
+      </c>
+      <c r="I49" s="2">
+        <v>14</v>
+      </c>
+      <c r="J49" s="2">
+        <v>52</v>
+      </c>
+      <c r="K49" s="2">
+        <v>58</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N49" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B50" s="2">
+        <v>16</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E50" s="2">
+        <v>24</v>
+      </c>
+      <c r="F50" s="2">
+        <v>15</v>
+      </c>
+      <c r="G50" s="2">
+        <v>31</v>
+      </c>
+      <c r="H50" s="2">
+        <v>55</v>
+      </c>
+      <c r="I50" s="2">
+        <v>16</v>
+      </c>
+      <c r="J50" s="2">
+        <v>7</v>
+      </c>
+      <c r="K50" s="2">
+        <v>20</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R50" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
saved work from home
</commit_message>
<xml_diff>
--- a/BWTracker.xlsx
+++ b/BWTracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="117">
   <si>
     <t>day</t>
   </si>
@@ -363,12 +363,15 @@
   </si>
   <si>
     <t>00:49:00</t>
+  </si>
+  <si>
+    <t>02:57:55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -571,23 +574,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -623,23 +609,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -817,7 +786,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:EL59"/>
+  <dimension ref="A1:EL60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -4513,6 +4482,62 @@
         <v>22</v>
       </c>
     </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" s="2">
+        <v>19</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E60" s="2">
+        <v>25</v>
+      </c>
+      <c r="F60" s="2">
+        <v>20</v>
+      </c>
+      <c r="G60" s="2">
+        <v>42</v>
+      </c>
+      <c r="H60" s="2">
+        <v>37</v>
+      </c>
+      <c r="I60" s="2">
+        <v>23</v>
+      </c>
+      <c r="J60" s="2">
+        <v>40</v>
+      </c>
+      <c r="K60" s="2">
+        <v>32</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N60" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P60" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R60" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>